<commit_message>
developing sustainable tourism goal, added data to layers, updated layers csv, working on updating functions
</commit_message>
<xml_diff>
--- a/prep/FIS/fis_reef_stock.xlsx
+++ b/prep/FIS/fis_reef_stock.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11310" yWindow="2250" windowWidth="27795" windowHeight="11820"/>
+    <workbookView xWindow="14550" yWindow="975" windowWidth="27795" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -539,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R1:V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,7 +845,7 @@
         <v>1.8333333333333335</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -862,7 +863,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>52</v>
       </c>
@@ -880,7 +881,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>34</v>
       </c>
@@ -898,7 +899,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>53</v>
       </c>
@@ -916,7 +917,7 @@
         <v>0.43333333333333335</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>55</v>
       </c>
@@ -933,8 +934,9 @@
         <f t="shared" si="0"/>
         <v>1.8000000000000003</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>54</v>
       </c>
@@ -951,8 +953,9 @@
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>55</v>
       </c>
@@ -970,7 +973,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>55</v>
       </c>
@@ -988,7 +991,7 @@
         <v>1.3666666666666667</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>55</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>0.8666666666666667</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>35</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>2.666666666666667</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>46</v>
       </c>
@@ -1042,7 +1045,7 @@
         <v>1.2666666666666668</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
updated FIS goal code
</commit_message>
<xml_diff>
--- a/prep/FIS/fis_reef_stock.xlsx
+++ b/prep/FIS/fis_reef_stock.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -540,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R1:V11"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +844,7 @@
         <v>1.8333333333333335</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -863,7 +862,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>52</v>
       </c>
@@ -881,7 +880,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>34</v>
       </c>
@@ -899,7 +898,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>53</v>
       </c>
@@ -917,7 +916,7 @@
         <v>0.43333333333333335</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>55</v>
       </c>
@@ -935,8 +934,9 @@
         <v>1.8000000000000003</v>
       </c>
       <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>54</v>
       </c>
@@ -954,8 +954,9 @@
         <v>0.76666666666666672</v>
       </c>
       <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>55</v>
       </c>
@@ -973,7 +974,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>55</v>
       </c>
@@ -991,7 +992,7 @@
         <v>1.3666666666666667</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>55</v>
       </c>
@@ -1009,7 +1010,7 @@
         <v>0.8666666666666667</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>35</v>
       </c>
@@ -1027,7 +1028,7 @@
         <v>2.666666666666667</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>46</v>
       </c>
@@ -1045,7 +1046,7 @@
         <v>1.2666666666666668</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>56</v>
       </c>
@@ -1062,6 +1063,28 @@
         <f t="shared" si="0"/>
         <v>1.9666666666666666</v>
       </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>